<commit_message>
I thought of a way to make it easier to exchange information between the GUI and the tester . The Tester could inherit from the GUI.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/PWR_Board_TestReportTemplate2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A6571-58C2-44D3-8BDB-98D7F21167DD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F4C470-EE20-404C-962D-A200B9C5A917}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="720" windowWidth="19440" windowHeight="15600" firstSheet="2" activeTab="6" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="-19320" yWindow="720" windowWidth="19440" windowHeight="15600" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -601,9 +601,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA788C9-474B-4068-A04A-775EAB4B4CD4}">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L84" sqref="L84"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +649,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -676,7 +676,7 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>1+A2</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -703,7 +703,7 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A15" si="2">1+A3</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -730,7 +730,7 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
@@ -757,7 +757,7 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -784,7 +784,7 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -811,7 +811,7 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -838,7 +838,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
@@ -865,7 +865,7 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -891,7 +891,7 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -917,7 +917,7 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -943,7 +943,7 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -969,7 +969,7 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -995,7 +995,7 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14.01</v>
+        <v>15.01</v>
       </c>
       <c r="B16" t="s">
         <v>59</v>
@@ -1050,7 +1050,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>A16+0.01</f>
-        <v>14.02</v>
+        <v>15.02</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
@@ -1080,7 +1080,7 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" ref="A18:A29" si="4">A17+0.01</f>
-        <v>14.03</v>
+        <v>15.03</v>
       </c>
       <c r="B18" t="s">
         <v>59</v>
@@ -1110,7 +1110,7 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="4"/>
-        <v>14.04</v>
+        <v>15.04</v>
       </c>
       <c r="B19" t="s">
         <v>59</v>
@@ -1140,7 +1140,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="4"/>
-        <v>14.049999999999999</v>
+        <v>15.049999999999999</v>
       </c>
       <c r="B20" t="s">
         <v>59</v>
@@ -1170,7 +1170,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="4"/>
-        <v>14.059999999999999</v>
+        <v>15.059999999999999</v>
       </c>
       <c r="B21" t="s">
         <v>59</v>
@@ -1200,7 +1200,7 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="4"/>
-        <v>14.069999999999999</v>
+        <v>15.069999999999999</v>
       </c>
       <c r="B22" t="s">
         <v>59</v>
@@ -1230,7 +1230,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="4"/>
-        <v>14.079999999999998</v>
+        <v>15.079999999999998</v>
       </c>
       <c r="B23" t="s">
         <v>59</v>
@@ -1260,7 +1260,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="4"/>
-        <v>14.089999999999998</v>
+        <v>15.089999999999998</v>
       </c>
       <c r="B24" t="s">
         <v>59</v>
@@ -1290,7 +1290,7 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="4"/>
-        <v>14.099999999999998</v>
+        <v>15.099999999999998</v>
       </c>
       <c r="B25" t="s">
         <v>59</v>
@@ -1320,7 +1320,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="4"/>
-        <v>14.109999999999998</v>
+        <v>15.109999999999998</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
@@ -1350,7 +1350,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>A26+0.01</f>
-        <v>14.119999999999997</v>
+        <v>15.119999999999997</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
@@ -1380,7 +1380,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="4"/>
-        <v>14.129999999999997</v>
+        <v>15.129999999999997</v>
       </c>
       <c r="B28" t="s">
         <v>59</v>
@@ -1410,7 +1410,7 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="4"/>
-        <v>14.139999999999997</v>
+        <v>15.139999999999997</v>
       </c>
       <c r="B29" t="s">
         <v>59</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>15.01</v>
+        <v>16.010000000000002</v>
       </c>
       <c r="B30" t="s">
         <v>60</v>
@@ -1469,7 +1469,7 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f>A30+0.01</f>
-        <v>15.02</v>
+        <v>16.020000000000003</v>
       </c>
       <c r="B31" t="s">
         <v>60</v>
@@ -1499,7 +1499,7 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f>A31+0.01</f>
-        <v>15.03</v>
+        <v>16.030000000000005</v>
       </c>
       <c r="B32" t="s">
         <v>60</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>16.010000000000002</v>
+        <v>17.010000000000002</v>
       </c>
       <c r="B33" t="s">
         <v>61</v>
@@ -1558,7 +1558,7 @@
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f>A33+0.01</f>
-        <v>16.020000000000003</v>
+        <v>17.020000000000003</v>
       </c>
       <c r="B34" t="s">
         <v>61</v>
@@ -1588,7 +1588,7 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" ref="A35:A46" si="5">A34+0.01</f>
-        <v>16.030000000000005</v>
+        <v>17.030000000000005</v>
       </c>
       <c r="B35" t="s">
         <v>61</v>
@@ -1618,7 +1618,7 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="5"/>
-        <v>16.040000000000006</v>
+        <v>17.040000000000006</v>
       </c>
       <c r="B36" t="s">
         <v>61</v>
@@ -1648,7 +1648,7 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="5"/>
-        <v>16.050000000000008</v>
+        <v>17.050000000000008</v>
       </c>
       <c r="B37" t="s">
         <v>61</v>
@@ -1678,7 +1678,7 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="5"/>
-        <v>16.060000000000009</v>
+        <v>17.060000000000009</v>
       </c>
       <c r="B38" t="s">
         <v>61</v>
@@ -1708,7 +1708,7 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="5"/>
-        <v>16.070000000000011</v>
+        <v>17.070000000000011</v>
       </c>
       <c r="B39" t="s">
         <v>61</v>
@@ -1738,7 +1738,7 @@
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="5"/>
-        <v>16.080000000000013</v>
+        <v>17.080000000000013</v>
       </c>
       <c r="B40" t="s">
         <v>61</v>
@@ -1768,7 +1768,7 @@
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="5"/>
-        <v>16.090000000000014</v>
+        <v>17.090000000000014</v>
       </c>
       <c r="B41" t="s">
         <v>61</v>
@@ -1798,7 +1798,7 @@
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="5"/>
-        <v>16.100000000000016</v>
+        <v>17.100000000000016</v>
       </c>
       <c r="B42" t="s">
         <v>61</v>
@@ -1828,7 +1828,7 @@
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="5"/>
-        <v>16.110000000000017</v>
+        <v>17.110000000000017</v>
       </c>
       <c r="B43" t="s">
         <v>61</v>
@@ -1858,7 +1858,7 @@
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="5"/>
-        <v>16.120000000000019</v>
+        <v>17.120000000000019</v>
       </c>
       <c r="B44" t="s">
         <v>61</v>
@@ -1888,7 +1888,7 @@
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="5"/>
-        <v>16.13000000000002</v>
+        <v>17.13000000000002</v>
       </c>
       <c r="B45" t="s">
         <v>61</v>
@@ -1918,7 +1918,7 @@
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="5"/>
-        <v>16.140000000000022</v>
+        <v>17.140000000000022</v>
       </c>
       <c r="B46" t="s">
         <v>61</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>17.010000000000002</v>
+        <v>18.010000000000002</v>
       </c>
       <c r="B47" t="s">
         <v>64</v>
@@ -1977,7 +1977,7 @@
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f>A47+0.01</f>
-        <v>17.020000000000003</v>
+        <v>18.020000000000003</v>
       </c>
       <c r="B48" t="s">
         <v>64</v>
@@ -2006,7 +2006,7 @@
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" ref="A49:A61" si="6">A48+0.01</f>
-        <v>17.030000000000005</v>
+        <v>18.030000000000005</v>
       </c>
       <c r="B49" t="s">
         <v>64</v>
@@ -2035,7 +2035,7 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="6"/>
-        <v>17.040000000000006</v>
+        <v>18.040000000000006</v>
       </c>
       <c r="B50" t="s">
         <v>64</v>
@@ -2064,7 +2064,7 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="6"/>
-        <v>17.050000000000008</v>
+        <v>18.050000000000008</v>
       </c>
       <c r="B51" t="s">
         <v>64</v>
@@ -2093,7 +2093,7 @@
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="6"/>
-        <v>17.060000000000009</v>
+        <v>18.060000000000009</v>
       </c>
       <c r="B52" t="s">
         <v>64</v>
@@ -2122,7 +2122,7 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="6"/>
-        <v>17.070000000000011</v>
+        <v>18.070000000000011</v>
       </c>
       <c r="B53" t="s">
         <v>64</v>
@@ -2151,7 +2151,7 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="6"/>
-        <v>17.080000000000013</v>
+        <v>18.080000000000013</v>
       </c>
       <c r="B54" t="s">
         <v>64</v>
@@ -2180,7 +2180,7 @@
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="6"/>
-        <v>17.090000000000014</v>
+        <v>18.090000000000014</v>
       </c>
       <c r="B55" t="s">
         <v>64</v>
@@ -2209,7 +2209,7 @@
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="6"/>
-        <v>17.100000000000016</v>
+        <v>18.100000000000016</v>
       </c>
       <c r="B56" t="s">
         <v>64</v>
@@ -2238,7 +2238,7 @@
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="6"/>
-        <v>17.110000000000017</v>
+        <v>18.110000000000017</v>
       </c>
       <c r="B57" t="s">
         <v>64</v>
@@ -2267,7 +2267,7 @@
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="6"/>
-        <v>17.120000000000019</v>
+        <v>18.120000000000019</v>
       </c>
       <c r="B58" t="s">
         <v>64</v>
@@ -2296,7 +2296,7 @@
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="6"/>
-        <v>17.13000000000002</v>
+        <v>18.13000000000002</v>
       </c>
       <c r="B59" t="s">
         <v>64</v>
@@ -2325,7 +2325,7 @@
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="6"/>
-        <v>17.140000000000022</v>
+        <v>18.140000000000022</v>
       </c>
       <c r="B60" t="s">
         <v>64</v>
@@ -2354,7 +2354,7 @@
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="6"/>
-        <v>17.150000000000023</v>
+        <v>18.150000000000023</v>
       </c>
       <c r="B61" t="s">
         <v>64</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>18.010000000000002</v>
+        <v>19.010000000000002</v>
       </c>
       <c r="B62" t="s">
         <v>59</v>
@@ -2411,7 +2411,7 @@
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f>A62+0.01</f>
-        <v>18.020000000000003</v>
+        <v>19.020000000000003</v>
       </c>
       <c r="B63" t="s">
         <v>59</v>
@@ -2440,7 +2440,7 @@
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" ref="A64:A75" si="7">A63+0.01</f>
-        <v>18.030000000000005</v>
+        <v>19.030000000000005</v>
       </c>
       <c r="B64" t="s">
         <v>59</v>
@@ -2469,7 +2469,7 @@
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="7"/>
-        <v>18.040000000000006</v>
+        <v>19.040000000000006</v>
       </c>
       <c r="B65" t="s">
         <v>59</v>
@@ -2498,7 +2498,7 @@
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="7"/>
-        <v>18.050000000000008</v>
+        <v>19.050000000000008</v>
       </c>
       <c r="B66" t="s">
         <v>59</v>
@@ -2527,7 +2527,7 @@
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="7"/>
-        <v>18.060000000000009</v>
+        <v>19.060000000000009</v>
       </c>
       <c r="B67" t="s">
         <v>59</v>
@@ -2556,7 +2556,7 @@
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" si="7"/>
-        <v>18.070000000000011</v>
+        <v>19.070000000000011</v>
       </c>
       <c r="B68" t="s">
         <v>59</v>
@@ -2585,7 +2585,7 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="7"/>
-        <v>18.080000000000013</v>
+        <v>19.080000000000013</v>
       </c>
       <c r="B69" t="s">
         <v>59</v>
@@ -2614,7 +2614,7 @@
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="7"/>
-        <v>18.090000000000014</v>
+        <v>19.090000000000014</v>
       </c>
       <c r="B70" t="s">
         <v>59</v>
@@ -2643,7 +2643,7 @@
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="7"/>
-        <v>18.100000000000016</v>
+        <v>19.100000000000016</v>
       </c>
       <c r="B71" t="s">
         <v>59</v>
@@ -2672,7 +2672,7 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="7"/>
-        <v>18.110000000000017</v>
+        <v>19.110000000000017</v>
       </c>
       <c r="B72" t="s">
         <v>59</v>
@@ -2701,7 +2701,7 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="7"/>
-        <v>18.120000000000019</v>
+        <v>19.120000000000019</v>
       </c>
       <c r="B73" t="s">
         <v>59</v>
@@ -2730,7 +2730,7 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="7"/>
-        <v>18.13000000000002</v>
+        <v>19.13000000000002</v>
       </c>
       <c r="B74" t="s">
         <v>59</v>
@@ -2759,7 +2759,7 @@
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="7"/>
-        <v>18.140000000000022</v>
+        <v>19.140000000000022</v>
       </c>
       <c r="B75" t="s">
         <v>59</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>19.010000000000002</v>
+        <v>20.010000000000002</v>
       </c>
       <c r="B76" t="s">
         <v>65</v>
@@ -2816,7 +2816,7 @@
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f>A76+0.01</f>
-        <v>19.020000000000003</v>
+        <v>20.020000000000003</v>
       </c>
       <c r="B77" t="s">
         <v>65</v>
@@ -2845,7 +2845,7 @@
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" ref="A78:A82" si="8">A77+0.01</f>
-        <v>19.030000000000005</v>
+        <v>20.030000000000005</v>
       </c>
       <c r="B78" t="s">
         <v>65</v>
@@ -2874,7 +2874,7 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="8"/>
-        <v>19.040000000000006</v>
+        <v>20.040000000000006</v>
       </c>
       <c r="B79" t="s">
         <v>65</v>
@@ -2903,7 +2903,7 @@
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="8"/>
-        <v>19.050000000000008</v>
+        <v>20.050000000000008</v>
       </c>
       <c r="B80" t="s">
         <v>65</v>
@@ -2932,7 +2932,7 @@
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="8"/>
-        <v>19.060000000000009</v>
+        <v>20.060000000000009</v>
       </c>
       <c r="B81" t="s">
         <v>65</v>
@@ -2961,7 +2961,7 @@
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="8"/>
-        <v>19.070000000000011</v>
+        <v>20.070000000000011</v>
       </c>
       <c r="B82" t="s">
         <v>65</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>20.010000000000002</v>
+        <v>21.01</v>
       </c>
       <c r="B83" t="s">
         <v>64</v>
@@ -3018,7 +3018,7 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f>A83+0.01</f>
-        <v>20.020000000000003</v>
+        <v>21.020000000000003</v>
       </c>
       <c r="B84" t="s">
         <v>64</v>
@@ -3047,7 +3047,7 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" ref="A85:A97" si="9">A84+0.01</f>
-        <v>20.030000000000005</v>
+        <v>21.030000000000005</v>
       </c>
       <c r="B85" t="s">
         <v>64</v>
@@ -3076,7 +3076,7 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="9"/>
-        <v>20.040000000000006</v>
+        <v>21.040000000000006</v>
       </c>
       <c r="B86" t="s">
         <v>64</v>
@@ -3105,7 +3105,7 @@
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="9"/>
-        <v>20.050000000000008</v>
+        <v>21.050000000000008</v>
       </c>
       <c r="B87" t="s">
         <v>64</v>
@@ -3134,7 +3134,7 @@
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="9"/>
-        <v>20.060000000000009</v>
+        <v>21.060000000000009</v>
       </c>
       <c r="B88" t="s">
         <v>64</v>
@@ -3163,7 +3163,7 @@
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="9"/>
-        <v>20.070000000000011</v>
+        <v>21.070000000000011</v>
       </c>
       <c r="B89" t="s">
         <v>64</v>
@@ -3192,7 +3192,7 @@
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="9"/>
-        <v>20.080000000000013</v>
+        <v>21.080000000000013</v>
       </c>
       <c r="B90" t="s">
         <v>64</v>
@@ -3221,7 +3221,7 @@
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="9"/>
-        <v>20.090000000000014</v>
+        <v>21.090000000000014</v>
       </c>
       <c r="B91" t="s">
         <v>64</v>
@@ -3250,7 +3250,7 @@
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="9"/>
-        <v>20.100000000000016</v>
+        <v>21.100000000000016</v>
       </c>
       <c r="B92" t="s">
         <v>64</v>
@@ -3279,7 +3279,7 @@
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f t="shared" si="9"/>
-        <v>20.110000000000017</v>
+        <v>21.110000000000017</v>
       </c>
       <c r="B93" t="s">
         <v>64</v>
@@ -3308,7 +3308,7 @@
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <f t="shared" si="9"/>
-        <v>20.120000000000019</v>
+        <v>21.120000000000019</v>
       </c>
       <c r="B94" t="s">
         <v>64</v>
@@ -3337,7 +3337,7 @@
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <f t="shared" si="9"/>
-        <v>20.13000000000002</v>
+        <v>21.13000000000002</v>
       </c>
       <c r="B95" t="s">
         <v>64</v>
@@ -3366,7 +3366,7 @@
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <f t="shared" si="9"/>
-        <v>20.140000000000022</v>
+        <v>21.140000000000022</v>
       </c>
       <c r="B96" t="s">
         <v>64</v>
@@ -3395,7 +3395,7 @@
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <f t="shared" si="9"/>
-        <v>20.150000000000023</v>
+        <v>21.150000000000023</v>
       </c>
       <c r="B97" t="s">
         <v>64</v>
@@ -4503,7 +4503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CEAD3C-E293-403D-9957-624DD4ECBBD6}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>

</xml_diff>